<commit_message>
create acc green banners modified
</commit_message>
<xml_diff>
--- a/pages/user_client_admin/Company Accounts.xlsx
+++ b/pages/user_client_admin/Company Accounts.xlsx
@@ -26,10 +26,10 @@
     <t>Accountant</t>
   </si>
   <si>
-    <t>Alison Pte Ltd</t>
+    <t>jp company</t>
   </si>
   <si>
-    <t>Jerry</t>
+    <t>accountant 1</t>
   </si>
 </sst>
 </file>
@@ -389,7 +389,7 @@
     </row>
     <row r="2" spans="1:3">
       <c r="A2">
-        <v>940385930</v>
+        <v>123</v>
       </c>
       <c r="B2" t="s">
         <v>3</v>

</xml_diff>